<commit_message>
Published state of ETDataset for deploy January 2023
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy/energy_hydrogen_biomass_gasification.xlsx
+++ b/nodes_source_analyses/energy/energy/energy_hydrogen_biomass_gasification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/energy/energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/nodes_source_analyses/energy/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559A96C7-5CF4-924E-9A19-6CA04B0EDEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF8FD21-FF29-6B4B-BD28-0CB244A0E34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="17500" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60160" yWindow="-18040" windowWidth="30080" windowHeight="16080" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -632,21 +632,6 @@
   </si>
   <si>
     <r>
-      <t>input.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>torrified_biomass_pellets</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>input</t>
     </r>
     <r>
@@ -711,6 +696,21 @@
   </si>
   <si>
     <t>See https://github.com/quintel/documentation/blob/master/general/cost_calculations.md#weighted-average-cost-of-capital</t>
+  </si>
+  <si>
+    <r>
+      <t>input.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>torrefied_biomass_pellets</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1754,7 +1754,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2010,6 +2010,7 @@
     <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="448">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3443,7 +3444,7 @@
   <dimension ref="A2:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
@@ -3564,8 +3565,8 @@
     <row r="13" spans="1:12" ht="17" thickBot="1">
       <c r="A13" s="13"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="149" t="s">
-        <v>170</v>
+      <c r="C13" s="175" t="s">
+        <v>177</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="103">
@@ -3609,7 +3610,7 @@
       <c r="A15" s="109"/>
       <c r="B15" s="110"/>
       <c r="C15" s="169" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>74</v>
@@ -3744,7 +3745,7 @@
     <row r="23" spans="1:11" ht="17" thickBot="1">
       <c r="B23" s="137"/>
       <c r="C23" s="170" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D23" s="139" t="s">
         <v>139</v>
@@ -3807,7 +3808,7 @@
       <c r="A26" s="142"/>
       <c r="B26" s="145"/>
       <c r="C26" s="170" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D26" s="139"/>
       <c r="E26" s="103">
@@ -3863,7 +3864,7 @@
       </c>
       <c r="H28" s="106"/>
       <c r="I28" s="163" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J28" s="112"/>
     </row>
@@ -4290,7 +4291,7 @@
     <row r="9" spans="1:20" ht="17" thickBot="1">
       <c r="B9" s="43"/>
       <c r="C9" s="150" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
@@ -4340,7 +4341,7 @@
     <row r="11" spans="1:20" ht="17" thickBot="1">
       <c r="B11" s="43"/>
       <c r="C11" s="168" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
@@ -5365,13 +5366,13 @@
     <row r="24" spans="2:7">
       <c r="B24" s="71"/>
       <c r="C24" s="171" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="71"/>
       <c r="C25" s="172" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="2:7">
@@ -5754,7 +5755,7 @@
         <v>74</v>
       </c>
       <c r="G73" s="65" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="2:7">

</xml_diff>